<commit_message>
add setter, Vehicle repository, Vehicle service
add setter, Vehicle repository, Vehicle service
</commit_message>
<xml_diff>
--- a/Car_UML/Car_UML.xlsx
+++ b/Car_UML/Car_UML.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
   <si>
     <t>Car</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -327,6 +327,98 @@
   </si>
   <si>
     <t>+getTotalKm()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+addVehicle(Vehicle)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+removeVehicle(Long)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+updateVehicle(Vehicle)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+findVehicleById(Long)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+getAllVehicle()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+findVehicleForStatus(VehicleStatus)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-vehicles : ArrayList&lt;Vehicle&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VehicleServiceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VehicleService &lt;&lt;interface&gt;&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setId(Long)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setCompany(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setModel(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setFactoryNumber(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setRegistNumber(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setColor(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setMakeYear(int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setTotalKm(int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setType(VehicleType)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+setStatus(VehicleStatus)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VehicleRepository &lt;&lt;interface&gt;&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VehicleJSONRepository</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+save(List&lt;Vehicle&gt;)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+load(List&lt;Vehicle&gt;)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -351,18 +443,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -456,10 +542,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -562,6 +648,112 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="5391150" y="247650"/>
           <a:ext cx="866775" cy="2428876"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="직선 화살표 연결선 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B19E9D-E5F5-4912-B7C4-4D9B2C5A391A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10010776" y="5476875"/>
+          <a:ext cx="9524" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="직선 화살표 연결선 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EE26FFA-A64F-4C74-9ADA-54324DC22A8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10001251" y="3343275"/>
+          <a:ext cx="9524" cy="619125"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -889,9 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1067,6 +1257,9 @@
       <c r="G10" s="5" t="s">
         <v>62</v>
       </c>
+      <c r="J10" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E11" s="5" t="s">
@@ -1075,167 +1268,258 @@
       <c r="G11" s="9" t="s">
         <v>74</v>
       </c>
+      <c r="J11" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="G13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="G14" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="G15" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E16" s="6"/>
+      <c r="E16" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G16" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J16" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E17" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="G17" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J17" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E18" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="G18" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J18" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E19" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="G19" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E20" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="G20" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E21" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="G21" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G22" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G23" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J23" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J24" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J25" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J26" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J27" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J28" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J29" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J33" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J34" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J35" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J36" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J37" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J38" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J39" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J40" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>20</v>
       </c>
@@ -1243,7 +1527,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>27</v>
       </c>
@@ -1251,7 +1535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>28</v>
       </c>
@@ -1259,7 +1543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>29</v>
       </c>
@@ -1267,12 +1551,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>30</v>
       </c>

</xml_diff>